<commit_message>
Additional files from last commit
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD689495-C175-4B32-BCE1-FCC62C79728E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D46BD-90B1-42A5-B112-0F7E5FF4282B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29745" yWindow="1425" windowWidth="27375" windowHeight="15225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61395" yWindow="2625" windowWidth="22140" windowHeight="13230" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="90">
   <si>
     <t>SoCDTtiNTY Share of Cargo Dist Transported that is New This Year</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Using IDEES data to better align with SYVbT</t>
+  </si>
+  <si>
+    <t>2024 (est.)</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -401,6 +404,7 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4672,23 +4676,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2EA77-52D5-4C8F-A27F-EB40305A89E1}">
-  <dimension ref="B3:J12"/>
+  <dimension ref="B3:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C4" s="7">
         <v>2018</v>
       </c>
@@ -4707,8 +4712,11 @@
       <c r="H4">
         <v>2023</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I4" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>64</v>
       </c>
@@ -4732,12 +4740,16 @@
       <c r="H5">
         <v>10547716</v>
       </c>
-      <c r="J5">
+      <c r="I5" s="13">
+        <f>H5*1.039</f>
+        <v>10959076.923999999</v>
+      </c>
+      <c r="K5">
         <f>AVERAGE(G5:H5)</f>
         <v>9905612.5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C7" s="7">
         <v>2018</v>
       </c>
@@ -4757,7 +4769,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -4781,7 +4793,7 @@
         <v>1467001</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -4808,7 +4820,7 @@
         <v>346986</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C11" s="7">
         <v>2018</v>
       </c>
@@ -4828,7 +4840,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>84</v>
       </c>
@@ -4873,6 +4885,7 @@
     <hyperlink ref="E11" r:id="rId14" display="https://www.acea.auto/files/Buses-by-fuel-type-full-year-2021.pdf" xr:uid="{FAAAD4F6-A61A-45BB-A02C-F0D70018057A}"/>
     <hyperlink ref="D11" r:id="rId15" display="https://www.acea.auto/files/ACEA_buses_by_fuel_type_full-year_2020.pdf" xr:uid="{D47C207F-C433-46C8-BA5F-916103C74EA7}"/>
     <hyperlink ref="C11" r:id="rId16" display="https://www.acea.auto/files/ACEA_buses_by_fuel_type_full-year_2019.pdf" xr:uid="{8EF9CE3B-FBC1-4815-B9A2-E0C84C8C73A0}"/>
+    <hyperlink ref="I4" r:id="rId17" xr:uid="{D948A403-B1EF-4144-B477-F70925E2DDBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4883,7 +4896,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5027,7 +5040,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5067,32 +5080,32 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="G2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(calcs!$D4:$F4)</f>
-        <v>3.8635512093079978E-2</v>
+        <f>AVERAGE(calcs!$C4:$F4)</f>
+        <v>4.234898604771057E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>